<commit_message>
High-Level Metrics, Device Monitoring, Device Registration, and Filtering implemented.
</commit_message>
<xml_diff>
--- a/Connected Office Dataset.xlsx
+++ b/Connected Office Dataset.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Semester 2\CMPG 323 - IT Developments\Project 5 - Reporting &amp; Monitoring\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marco\Documents\Repos\CMPG-323-Project-5---35314389\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDF2E506-73F6-48C0-BDFA-A739727EDDDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1FB60DD-A06A-4F8F-99AE-D2A23775281B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4269" yWindow="3909" windowWidth="23305" windowHeight="11057" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zone" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="101">
   <si>
     <t>ID</t>
   </si>
@@ -141,9 +141,6 @@
     <t>Is Active</t>
   </si>
   <si>
-    <t>Date Installe</t>
-  </si>
-  <si>
     <t>D01</t>
   </si>
   <si>
@@ -334,13 +331,19 @@
   </si>
   <si>
     <t>TotalDevices</t>
+  </si>
+  <si>
+    <t>Date Installed</t>
+  </si>
+  <si>
+    <t>Online vs Offline</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -375,6 +378,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -384,7 +393,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -516,11 +525,50 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -529,10 +577,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
@@ -550,6 +596,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -866,8 +915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -888,8 +937,8 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="20" t="s">
-        <v>98</v>
+      <c r="D1" s="18" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.4">
@@ -902,8 +951,8 @@
       <c r="C2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="16">
-        <f>COUNTIF(Device!D2:D10,"Boilermaker Room")</f>
+      <c r="D2" s="14">
+        <f>COUNTIF(Device!D2:D10,"Z01")</f>
         <v>1</v>
       </c>
     </row>
@@ -917,8 +966,8 @@
       <c r="C3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="16">
-        <f>COUNTIF(Device!D2:D10,"Terrazzo")</f>
+      <c r="D3" s="14">
+        <f>COUNTIF(Device!D2:D10,"Z02")</f>
         <v>1</v>
       </c>
     </row>
@@ -932,8 +981,8 @@
       <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="16">
-        <f>COUNTIF(Device!D2:D10,"Safety Office")</f>
+      <c r="D4" s="14">
+        <f>COUNTIF(Device!D2:D10,"Z03")</f>
         <v>1</v>
       </c>
     </row>
@@ -947,8 +996,8 @@
       <c r="C5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="16">
-        <f>COUNTIF(Device!D2:D10,"Stucco Mason Building")</f>
+      <c r="D5" s="14">
+        <f>COUNTIF(Device!D2:D10,"Z04")</f>
         <v>2</v>
       </c>
     </row>
@@ -962,8 +1011,8 @@
       <c r="C6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="16">
-        <f>COUNTIF(Device!D2:D10,"Iron Workshop")</f>
+      <c r="D6" s="14">
+        <f>COUNTIF(Device!D2:D10,"Z05")</f>
         <v>0</v>
       </c>
     </row>
@@ -977,8 +1026,8 @@
       <c r="C7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="16">
-        <f>COUNTIF(Device!D2:D10,"Labor Office")</f>
+      <c r="D7" s="14">
+        <f>COUNTIF(Device!D2:D10,"Z06")</f>
         <v>1</v>
       </c>
     </row>
@@ -992,8 +1041,8 @@
       <c r="C8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="16">
-        <f>COUNTIF(Device!D2:D10,"Environmental Office")</f>
+      <c r="D8" s="14">
+        <f>COUNTIF(Device!D2:D10,"Z07")</f>
         <v>1</v>
       </c>
     </row>
@@ -1007,8 +1056,8 @@
       <c r="C9" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="16">
-        <f>COUNTIF(Device!D2:D10,"Tile Setting Bench")</f>
+      <c r="D9" s="14">
+        <f>COUNTIF(Device!D2:D10,"Z08")</f>
         <v>1</v>
       </c>
     </row>
@@ -1022,8 +1071,8 @@
       <c r="C10" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="16">
-        <f>COUNTIF(Device!D2:D10,"Linemen Assembly")</f>
+      <c r="D10" s="14">
+        <f>COUNTIF(Device!D2:D10,"Z09")</f>
         <v>1</v>
       </c>
     </row>
@@ -1034,10 +1083,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08439157-EFCA-47CB-8108-F53748A39E5E}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1049,9 +1098,10 @@
     <col min="5" max="5" width="12.69140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.15234375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.84375" customWidth="1"/>
+    <col min="8" max="8" width="14.53515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1067,221 +1117,261 @@
       <c r="E1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A2" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>37</v>
-      </c>
       <c r="C2" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" s="20">
+        <v>43855</v>
+      </c>
+      <c r="H2" s="14" t="str">
+        <f>IF(E2="In Operation", "Online", "Offline")</f>
+        <v>Online</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F2" s="10" t="b">
+      <c r="B3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="9" t="b">
         <v>1</v>
       </c>
-      <c r="G2" s="11">
-        <v>43855</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A3" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="G3" s="20">
+        <v>44229</v>
+      </c>
+      <c r="H3" s="14" t="str">
+        <f t="shared" ref="H3:H10" si="0">IF(E3="In Operation", "Online", "Offline")</f>
+        <v>Offline</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A4" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" s="20">
+        <v>44541</v>
+      </c>
+      <c r="H4" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>Online</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" s="20">
+        <v>44641</v>
+      </c>
+      <c r="H5" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>Online</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" s="20">
+        <v>44641</v>
+      </c>
+      <c r="H6" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>Offline</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A7" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F3" s="10" t="b">
+      <c r="F7" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="G7" s="20">
+        <v>44333</v>
+      </c>
+      <c r="H7" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>Offline</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A8" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="9" t="b">
         <v>1</v>
       </c>
-      <c r="G3" s="11">
-        <v>44229</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A4" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F4" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="G4" s="11">
-        <v>44541</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A5" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F5" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="G5" s="11">
-        <v>44641</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A6" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="F6" s="10" t="b">
+      <c r="G8" s="20">
+        <v>44409</v>
+      </c>
+      <c r="H8" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>Online</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A9" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="G6" s="11">
-        <v>44641</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A7" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F7" s="10" t="b">
+      <c r="G9" s="20">
+        <v>44434</v>
+      </c>
+      <c r="H9" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>Offline</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A10" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F10" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="G7" s="11">
-        <v>44333</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A8" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F8" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="G8" s="11">
-        <v>44409</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A9" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="F9" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="G9" s="11">
-        <v>44434</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A10" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="F10" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="G10" s="11">
+      <c r="G10" s="21">
         <v>44584</v>
       </c>
+      <c r="H10" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>Offline</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1307,116 +1397,116 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>99</v>
+      <c r="D1" s="10" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="32.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="C2" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="D2" s="16">
+      <c r="D2" s="14">
         <f>COUNT('Sub-Category'!E2:E6)</f>
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="77.599999999999994" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="C3" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="D3" s="16">
+      <c r="D3" s="14">
         <f>COUNTIF(Device!C2:C10,"Computing")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A4" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="C4" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="C4" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="D4" s="16">
+      <c r="D4" s="14">
         <f>COUNTIF(Device!C2:C10,"Communicating")</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="C5" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="C5" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="D5" s="16">
+      <c r="D5" s="14">
         <f>COUNTIF(Device!C2:C10,"Actuating")</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="30.9" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="C6" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="C6" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="D6" s="16">
+      <c r="D6" s="14">
         <f>COUNTIF(Device!C2:C10,"Security")</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A7" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="C7" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="C7" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="D7" s="16">
+      <c r="D7" s="14">
         <f>COUNTIF(Device!C2:C10,"Energy")</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A8" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="C8" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="C8" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="D8" s="16">
+      <c r="D8" s="14">
         <f>COUNTIF(Device!C2:C10,"Privacy")</f>
         <v>0</v>
       </c>
@@ -1430,8 +1520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC903D32-5F9E-4786-89D6-996B7E75E220}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1451,103 +1541,103 @@
         <v>31</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="E1" s="20" t="s">
-        <v>97</v>
+      <c r="E1" s="18" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="E2" s="16">
-        <f>COUNTIF(Device!C2:C10,"Camera")</f>
+      <c r="E2" s="14">
+        <f>COUNTIF(Device!C2:C10,"SC01")</f>
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="E3" s="16">
-        <f>COUNTIF(Device!C2:C10,"Temperature Sensor")</f>
+      <c r="E3" s="14">
+        <f>COUNTIF(Device!C2:C10,"SC02")</f>
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="E4" s="16">
-        <f>COUNTIF(Device!C2:C10,"Motion Sensor")</f>
+      <c r="E4" s="14">
+        <f>COUNTIF(Device!C2:C10,"SC03")</f>
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="E5" s="16">
-        <f>COUNTIF(Device!C2:C10,"Access Control")</f>
-        <v>2</v>
+      <c r="E5" s="14">
+        <f>COUNTIF(Device!C2:C10,"SC04")</f>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="E6" s="16">
-        <f>COUNTIF(Device!C2:C10,"Speed Sensor")</f>
-        <v>1</v>
+      <c r="E6" s="14">
+        <f>COUNTIF(Device!C2:C10,"SC05")</f>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>